<commit_message>
added defect tracker file
</commit_message>
<xml_diff>
--- a/Internship_artifacts/RuhiParveen_AI_Visa_Defect_Tracker.xlsx
+++ b/Internship_artifacts/RuhiParveen_AI_Visa_Defect_Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x280\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bvree\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FA9DAB-5BA0-40AE-8908-BEF278E4A397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{88C213D3-C04B-4D71-BF6C-4B8F2E2DCAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defect Tracker" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t>Sl No</t>
   </si>
@@ -86,15 +86,127 @@
   </si>
   <si>
     <t>UI alignment and text formatting issues</t>
+  </si>
+  <si>
+    <t>Type of Defect</t>
+  </si>
+  <si>
+    <t>Action Taken Date</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Algorithmic</t>
+  </si>
+  <si>
+    <t>Logic</t>
+  </si>
+  <si>
+    <t>UI/Validation</t>
+  </si>
+  <si>
+    <t>Error Handling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performance </t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Action Taken</t>
+  </si>
+  <si>
+    <t>Improved image preprocessing, added noise removal</t>
+  </si>
+  <si>
+    <t>Implemented data validation checks and default handling for missing fields</t>
+  </si>
+  <si>
+    <t>Re-evaluated feature selection and retrained model with updated dataset</t>
+  </si>
+  <si>
+    <t>Status(Opened/Closed)</t>
+  </si>
+  <si>
+    <t>Corrected calculation logic and added boundary condition check</t>
+  </si>
+  <si>
+    <t>Fixed API response binding and UI state update logic</t>
+  </si>
+  <si>
+    <t>Added file type, size validation, and proper error messages</t>
+  </si>
+  <si>
+    <t>Optimized database queries and enabled caching for frequent requests</t>
+  </si>
+  <si>
+    <t>Implemented auto-refresh and backend trigger after retraining</t>
+  </si>
+  <si>
+    <t>Fixed backend mapping logic between prediction output and rejection messages</t>
+  </si>
+  <si>
+    <t>Adjusted CSS styles and tested across screen resolutions</t>
+  </si>
+  <si>
+    <t>Prediction accuracy stabilized after fix</t>
+  </si>
+  <si>
+    <t>Model performance now consistent with validation results</t>
+  </si>
+  <si>
+    <t>Negative values eliminated</t>
+  </si>
+  <si>
+    <t>Result now displayed correctly on UI</t>
+  </si>
+  <si>
+    <t>Invalid uploads are now blocked with user alerts</t>
+  </si>
+  <si>
+    <t>Response time improved during high traffic</t>
+  </si>
+  <si>
+    <t>Dashboard reflects latest model results</t>
+  </si>
+  <si>
+    <t>Correct rejection reason now shown</t>
+  </si>
+  <si>
+    <t>UI looks consistent across devices</t>
+  </si>
+  <si>
+    <t>OCR accuracy improved, extraction errors reduced</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -127,11 +239,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,206 +557,386 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="60.7109375" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="50.5546875" customWidth="1"/>
+    <col min="4" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="52.77734375" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" customWidth="1"/>
+    <col min="10" max="10" width="40.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="5">
         <v>45988</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="F2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="5">
+        <v>45989</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>45989</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="5">
+        <v>45990</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="F3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="5">
+        <v>45991</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <v>45997</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="F4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="5">
+        <v>45998</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="5">
         <v>46001</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="F5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="5">
+        <v>46002</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="5">
         <v>46003</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="F6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="5">
+        <v>46004</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="5">
         <v>46008</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="F7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="5">
+        <v>46009</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="5">
         <v>46017</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="F8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="5">
+        <v>46018</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="5">
         <v>46024</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="F9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="5">
+        <v>46025</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="5">
         <v>46031</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="F10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="5">
+        <v>46032</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="5">
         <v>46038</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="F11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="5">
+        <v>46039</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>